<commit_message>
prep ozone VTZP MS-CASPT2
</commit_message>
<xml_diff>
--- a/ozone/multistate/ANO-RCC-VTZP/ozone_106.00/ozone_106.00_energies.xlsx
+++ b/ozone/multistate/ANO-RCC-VTZP/ozone_106.00/ozone_106.00_energies.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.5080600293</v>
+        <v>-0.5607738878</v>
       </c>
       <c r="C2" t="n">
-        <v>-224.77743158</v>
+        <v>-224.72799182</v>
       </c>
       <c r="D2" t="n">
-        <v>-225.28549161</v>
+        <v>-225.28876571</v>
       </c>
       <c r="E2" t="n">
         <v>-224.502770001</v>
@@ -481,13 +481,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.4907663078</v>
+        <v>-0.5693531088</v>
       </c>
       <c r="C3" t="n">
-        <v>-224.73544516</v>
+        <v>-224.66963371</v>
       </c>
       <c r="D3" t="n">
-        <v>-225.22621147</v>
+        <v>-225.23898681</v>
       </c>
       <c r="E3" t="n">
         <v>-224.502770001</v>
@@ -500,13 +500,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.4908578798</v>
+        <v>-0.5696708344</v>
       </c>
       <c r="C4" t="n">
-        <v>-224.70884307</v>
+        <v>-224.63670635</v>
       </c>
       <c r="D4" t="n">
-        <v>-225.19970095</v>
+        <v>-225.20637719</v>
       </c>
       <c r="E4" t="n">
         <v>-224.502770001</v>

</xml_diff>